<commit_message>
Functions were created and modified
kin_chain_steps was created to find and index the vel and acc of each step along the kinematic chain.
</commit_message>
<xml_diff>
--- a/Masters Thesis Project/userProfile.xlsx
+++ b/Masters Thesis Project/userProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MT/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MT/Documents/GitHub/QualisysMotionCapture/Masters Thesis Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3E03887-29DC-1C42-BF0A-AC79153F2F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D7A22A-6E13-D540-9F70-54634E733C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="14200" xr2:uid="{FB65B791-6972-E743-882F-9E844BA861C0}"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="13820" xr2:uid="{FB65B791-6972-E743-882F-9E844BA861C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,16 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Jon Matthis</t>
-  </si>
-  <si>
-    <t>Matheus Turra</t>
-  </si>
-  <si>
     <t>Height (mm)</t>
   </si>
   <si>
     <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>JSM</t>
+  </si>
+  <si>
+    <t>MFBT</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -412,15 +412,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1778</v>
@@ -431,7 +431,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1778</v>

</xml_diff>